<commit_message>
trips by mode data
</commit_message>
<xml_diff>
--- a/data/mobility/OD_ageragates_of_zones.xlsx
+++ b/data/mobility/OD_ageragates_of_zones.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="BUS TRIPS" sheetId="1" r:id="rId1"/>
+    <sheet name="TRIPS BY MODE" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="35">
   <si>
     <t>OD</t>
   </si>
@@ -84,6 +85,51 @@
   </si>
   <si>
     <t>13,14,15,16,17,18,19,20</t>
+  </si>
+  <si>
+    <t>Médina-SYBA</t>
+  </si>
+  <si>
+    <t>Azli-Massira</t>
+  </si>
+  <si>
+    <t>Mhamid and Others</t>
+  </si>
+  <si>
+    <t>Pedestrians</t>
+  </si>
+  <si>
+    <t>Cars</t>
+  </si>
+  <si>
+    <t>2-wheels</t>
+  </si>
+  <si>
+    <t>Bus + Taxis</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Daily generated trips by mode in aggregates of zones (2008)</t>
+  </si>
+  <si>
+    <t>ORIGINAL OD</t>
+  </si>
+  <si>
+    <t>↑</t>
+  </si>
+  <si>
+    <t>Medina-SYBA</t>
+  </si>
+  <si>
+    <t>1,2,3,4,8</t>
+  </si>
+  <si>
+    <t>12,24,27,21,22,23</t>
+  </si>
+  <si>
+    <t>13,14,15,16,17,18,19,20,25,26</t>
   </si>
 </sst>
 </file>
@@ -128,7 +174,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +199,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -166,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -197,15 +255,55 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -487,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,21 +608,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -557,11 +655,11 @@
       <c r="J2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -598,10 +696,10 @@
       <c r="M3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="N3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="13"/>
+      <c r="O3" s="14"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -638,10 +736,10 @@
       <c r="M4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="N4" s="13" t="s">
+      <c r="N4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="13"/>
+      <c r="O4" s="14"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -678,10 +776,10 @@
       <c r="M5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="13" t="s">
+      <c r="N5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="O5" s="13"/>
+      <c r="O5" s="14"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -718,10 +816,10 @@
       <c r="M6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="13">
+      <c r="N6" s="14">
         <v>8</v>
       </c>
-      <c r="O6" s="13"/>
+      <c r="O6" s="14"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -758,10 +856,10 @@
       <c r="M7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N7" s="13" t="s">
+      <c r="N7" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="O7" s="13"/>
+      <c r="O7" s="14"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -798,10 +896,10 @@
       <c r="M8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N8" s="13" t="s">
+      <c r="N8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="O8" s="13"/>
+      <c r="O8" s="14"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
@@ -838,10 +936,10 @@
       <c r="M9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N9" s="13" t="s">
+      <c r="N9" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="O9" s="13"/>
+      <c r="O9" s="14"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -878,10 +976,10 @@
       <c r="M10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N10" s="13" t="s">
+      <c r="N10" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="13"/>
+      <c r="O10" s="14"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
@@ -890,18 +988,460 @@
         <v>99713</v>
       </c>
     </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="D12" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="11"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D13" s="27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="12"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="25">
+        <v>1005</v>
+      </c>
+      <c r="C17" s="6">
+        <v>3705</v>
+      </c>
+      <c r="D17" s="6">
+        <v>6300</v>
+      </c>
+      <c r="E17" s="6">
+        <v>4025</v>
+      </c>
+      <c r="F17" s="6">
+        <v>5010</v>
+      </c>
+      <c r="G17" s="6">
+        <v>16320</v>
+      </c>
+      <c r="H17" s="12">
+        <v>6420</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="25">
+        <v>160</v>
+      </c>
+      <c r="D18" s="6">
+        <v>460</v>
+      </c>
+      <c r="E18" s="6">
+        <v>3230</v>
+      </c>
+      <c r="F18" s="6">
+        <v>830</v>
+      </c>
+      <c r="G18" s="6">
+        <v>3210</v>
+      </c>
+      <c r="H18" s="12">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="25">
+        <v>620</v>
+      </c>
+      <c r="E19" s="6">
+        <v>2665</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1710</v>
+      </c>
+      <c r="G19" s="6">
+        <v>3565</v>
+      </c>
+      <c r="H19" s="12">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="25">
+        <v>565</v>
+      </c>
+      <c r="F20" s="6">
+        <v>2895</v>
+      </c>
+      <c r="G20" s="6">
+        <v>5030</v>
+      </c>
+      <c r="H20" s="12">
+        <v>2525</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="25">
+        <v>335</v>
+      </c>
+      <c r="G21" s="6">
+        <v>4995</v>
+      </c>
+      <c r="H21" s="12">
+        <v>2225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="25">
+        <v>1555</v>
+      </c>
+      <c r="H22" s="12">
+        <v>5240</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="26">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="19"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="N7:O7"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="N9:O9"/>
     <mergeCell ref="N10:O10"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="20">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C3" s="20">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D3" s="20">
+        <v>0.24</v>
+      </c>
+      <c r="E3" s="20">
+        <v>0.06</v>
+      </c>
+      <c r="F3" s="21">
+        <f>SUM(B3:E3)</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="20">
+        <v>0.45</v>
+      </c>
+      <c r="C4" s="20">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D4" s="20">
+        <v>0.24</v>
+      </c>
+      <c r="E4" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="F4" s="21">
+        <f t="shared" ref="F4:F7" si="0">SUM(B4:E4)</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="20">
+        <v>0.26</v>
+      </c>
+      <c r="D5" s="20">
+        <v>0.17</v>
+      </c>
+      <c r="E5" s="20">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F5" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="14"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="20">
+        <v>0.63</v>
+      </c>
+      <c r="C6" s="20">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D6" s="20">
+        <v>0.18</v>
+      </c>
+      <c r="E6" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="F6" s="21">
+        <f t="shared" si="0"/>
+        <v>0.98</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="14"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="21">
+        <v>0.64</v>
+      </c>
+      <c r="C7" s="21">
+        <v>0.12</v>
+      </c>
+      <c r="D7" s="21">
+        <v>0.21</v>
+      </c>
+      <c r="E7" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="F7" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="29"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="20">
+        <f>AVERAGE(B3:B7)</f>
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="C8" s="20">
+        <f>AVERAGE(C3:C7)</f>
+        <v>0.188</v>
+      </c>
+      <c r="D8" s="20">
+        <f t="shared" ref="D8:E8" si="1">AVERAGE(D3:D7)</f>
+        <v>0.20800000000000002</v>
+      </c>
+      <c r="E8" s="20">
+        <f t="shared" si="1"/>
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F8" s="21">
+        <f>SUM(B8:E8)</f>
+        <v>0.996</v>
+      </c>
+      <c r="J8" s="28"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:L8"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
new matrices and a generator in gaml
</commit_message>
<xml_diff>
--- a/data/mobility/OD_ageragates_of_zones.xlsx
+++ b/data/mobility/OD_ageragates_of_zones.xlsx
@@ -57,12 +57,6 @@
     <t>Guéliz-Hivernage</t>
   </si>
   <si>
-    <t>Médina</t>
-  </si>
-  <si>
-    <t>Other zones</t>
-  </si>
-  <si>
     <t>Mapping agregate-zones</t>
   </si>
   <si>
@@ -130,6 +124,12 @@
   </si>
   <si>
     <t>13,14,15,16,17,18,19,20,25,26</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Gueliz_Hiv</t>
   </si>
 </sst>
 </file>
@@ -224,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -259,15 +259,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -281,22 +272,34 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -588,38 +591,37 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
       <c r="M1" s="13"/>
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
@@ -629,13 +631,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>5</v>
@@ -650,16 +652,16 @@
         <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
+      <c r="M2" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -696,10 +698,10 @@
       <c r="M3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" s="14"/>
+      <c r="N3" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="28"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -736,14 +738,14 @@
       <c r="M4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="N4" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="O4" s="14"/>
+      <c r="N4" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="28"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>9</v>
+      <c r="A5" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="B5" s="6">
         <v>3150</v>
@@ -773,13 +775,13 @@
         <f t="shared" si="0"/>
         <v>9436</v>
       </c>
-      <c r="M5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N5" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="O5" s="14"/>
+      <c r="M5" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="28"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -816,10 +818,10 @@
       <c r="M6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="28">
         <v>8</v>
       </c>
-      <c r="O6" s="14"/>
+      <c r="O6" s="28"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -856,10 +858,10 @@
       <c r="M7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N7" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="O7" s="14"/>
+      <c r="N7" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" s="28"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -896,10 +898,10 @@
       <c r="M8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N8" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="O8" s="14"/>
+      <c r="N8" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8" s="28"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
@@ -936,14 +938,14 @@
       <c r="M9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N9" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="O9" s="14"/>
+      <c r="N9" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="O9" s="28"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B10" s="6">
         <v>1092</v>
@@ -974,12 +976,12 @@
         <v>4993</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N10" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="O10" s="14"/>
+        <v>33</v>
+      </c>
+      <c r="N10" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10" s="28"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
@@ -990,42 +992,42 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="D12" s="27" t="s">
-        <v>30</v>
+      <c r="D12" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D13" s="27" t="s">
-        <v>30</v>
+      <c r="D13" s="23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
+      <c r="A15" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>9</v>
+      <c r="D16" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>5</v>
@@ -1046,7 +1048,7 @@
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="25">
+      <c r="B17" s="21">
         <v>1005</v>
       </c>
       <c r="C17" s="6">
@@ -1073,7 +1075,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="6"/>
-      <c r="C18" s="25">
+      <c r="C18" s="21">
         <v>160</v>
       </c>
       <c r="D18" s="6">
@@ -1093,12 +1095,12 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>9</v>
+      <c r="A19" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="25">
+      <c r="D19" s="21">
         <v>620</v>
       </c>
       <c r="E19" s="6">
@@ -1121,7 +1123,7 @@
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="25">
+      <c r="E20" s="21">
         <v>565</v>
       </c>
       <c r="F20" s="6">
@@ -1142,7 +1144,7 @@
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="25">
+      <c r="F21" s="21">
         <v>335</v>
       </c>
       <c r="G21" s="6">
@@ -1161,7 +1163,7 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="25">
+      <c r="G22" s="21">
         <v>1555</v>
       </c>
       <c r="H22" s="12">
@@ -1178,20 +1180,20 @@
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
-      <c r="H23" s="26">
+      <c r="H23" s="22">
         <v>1515</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="19"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1217,7 +1219,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,205 +1234,205 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="A1" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
+      <c r="J2" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="20">
+        <v>18</v>
+      </c>
+      <c r="B3" s="17">
         <v>0.56000000000000005</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="17">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="17">
         <v>0.24</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="17">
         <v>0.06</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="18">
         <f>SUM(B3:E3)</f>
         <v>1</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="14"/>
+        <v>29</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="28"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="17">
         <v>0.45</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="17">
         <v>0.28000000000000003</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="17">
         <v>0.24</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="17">
         <v>0.03</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="18">
         <f t="shared" ref="F4:F7" si="0">SUM(B4:E4)</f>
         <v>1</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="14"/>
+      <c r="K4" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="28"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="17">
         <v>0.5</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="17">
         <v>0.26</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="17">
         <v>0.17</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="17">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="18">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="14"/>
+      <c r="K5" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="28"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="20">
+        <v>19</v>
+      </c>
+      <c r="B6" s="17">
         <v>0.63</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="17">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="17">
         <v>0.18</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="17">
         <v>0.03</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="18">
         <f t="shared" si="0"/>
         <v>0.98</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" s="14"/>
+        <v>19</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="28"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="21">
+        <v>20</v>
+      </c>
+      <c r="B7" s="18">
         <v>0.64</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="18">
         <v>0.12</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="18">
         <v>0.21</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="18">
         <v>0.03</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="18">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J7" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="29"/>
+      <c r="J7" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" s="30"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="20">
+        <v>25</v>
+      </c>
+      <c r="B8" s="17">
         <f>AVERAGE(B3:B7)</f>
         <v>0.55600000000000005</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="17">
         <f>AVERAGE(C3:C7)</f>
         <v>0.188</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="17">
         <f t="shared" ref="D8:E8" si="1">AVERAGE(D3:D7)</f>
         <v>0.20800000000000002</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="17">
         <f t="shared" si="1"/>
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="18">
         <f>SUM(B8:E8)</f>
         <v>0.996</v>
       </c>
-      <c r="J8" s="28"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>